<commit_message>
Filtering real approved data
</commit_message>
<xml_diff>
--- a/apps/dataset/Database.xlsx
+++ b/apps/dataset/Database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="overview" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="66">
   <si>
     <t>Nome etapa</t>
   </si>
@@ -203,6 +203,18 @@
   </si>
   <si>
     <t>zz9 referente descrição de zz8</t>
+  </si>
+  <si>
+    <t>2.0.7.04</t>
+  </si>
+  <si>
+    <t>1.6.4.02</t>
+  </si>
+  <si>
+    <t>TXRAIL-USB-RESISTÊNCIA</t>
+  </si>
+  <si>
+    <t>TXRAIL-USB-VALIDAÇÃO</t>
   </si>
 </sst>
 </file>
@@ -218,7 +230,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,8 +243,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -268,11 +286,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -280,12 +342,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -328,8 +402,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A3:V33" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A3:V33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A3:V88" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A3:V88"/>
   <tableColumns count="22">
     <tableColumn id="1" name="VERSAO SW"/>
     <tableColumn id="2" name="VERSAO FW"/>
@@ -671,21 +745,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
     </row>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -817,30 +891,30 @@
       </c>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -973,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:V33"/>
+  <dimension ref="A2:V88"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,30 +1074,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -2195,7 +2269,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -2230,6 +2304,2396 @@
         <v>52</v>
       </c>
       <c r="N33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="9">
+        <v>211</v>
+      </c>
+      <c r="C34" s="9">
+        <v>19130584</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="9">
+        <v>110</v>
+      </c>
+      <c r="F34" s="9">
+        <v>20018589</v>
+      </c>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9">
+        <v>6952101001</v>
+      </c>
+      <c r="K34" s="10">
+        <v>43990</v>
+      </c>
+      <c r="L34" s="11">
+        <v>0.53003472222222225</v>
+      </c>
+      <c r="M34" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="N34" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
+      <c r="T34" s="4"/>
+      <c r="U34" s="4"/>
+      <c r="V34" s="4"/>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="12">
+        <v>211</v>
+      </c>
+      <c r="C35" s="12">
+        <v>19130584</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E35" s="12">
+        <v>110</v>
+      </c>
+      <c r="F35" s="12">
+        <v>20018589</v>
+      </c>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12">
+        <v>6952101001</v>
+      </c>
+      <c r="K35" s="13">
+        <v>43990</v>
+      </c>
+      <c r="L35" s="14">
+        <v>0.53070601851851851</v>
+      </c>
+      <c r="M35" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="N35" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4"/>
+      <c r="S35" s="4"/>
+      <c r="T35" s="4"/>
+      <c r="U35" s="4"/>
+      <c r="V35" s="4"/>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" s="9">
+        <v>211</v>
+      </c>
+      <c r="C36" s="9">
+        <v>19130584</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" s="9">
+        <v>104</v>
+      </c>
+      <c r="F36" s="9">
+        <v>20018589</v>
+      </c>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9">
+        <v>6952101001</v>
+      </c>
+      <c r="K36" s="10">
+        <v>43990</v>
+      </c>
+      <c r="L36" s="11">
+        <v>0.53070601851851851</v>
+      </c>
+      <c r="M36" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="N36" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="4"/>
+      <c r="S36" s="4"/>
+      <c r="T36" s="4"/>
+      <c r="U36" s="4"/>
+      <c r="V36" s="4"/>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" s="12">
+        <v>211</v>
+      </c>
+      <c r="C37" s="12">
+        <v>19130584</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" s="12">
+        <v>104</v>
+      </c>
+      <c r="F37" s="12">
+        <v>20018589</v>
+      </c>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12">
+        <v>6952101001</v>
+      </c>
+      <c r="K37" s="13">
+        <v>43990</v>
+      </c>
+      <c r="L37" s="14">
+        <v>0.53070601851851851</v>
+      </c>
+      <c r="M37" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N37" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4"/>
+      <c r="S37" s="4"/>
+      <c r="T37" s="4"/>
+      <c r="U37" s="4"/>
+      <c r="V37" s="4"/>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="9">
+        <v>211</v>
+      </c>
+      <c r="C38" s="9">
+        <v>12312274</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" s="9">
+        <v>104</v>
+      </c>
+      <c r="F38" s="9">
+        <v>20018589</v>
+      </c>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9">
+        <v>6952101001</v>
+      </c>
+      <c r="K38" s="10">
+        <v>43990</v>
+      </c>
+      <c r="L38" s="11">
+        <v>0.64475694444444442</v>
+      </c>
+      <c r="M38" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="N38" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="4"/>
+      <c r="S38" s="4"/>
+      <c r="T38" s="4"/>
+      <c r="U38" s="4"/>
+      <c r="V38" s="4"/>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" s="12">
+        <v>211</v>
+      </c>
+      <c r="C39" s="12">
+        <v>19130584</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E39" s="12">
+        <v>104</v>
+      </c>
+      <c r="F39" s="12">
+        <v>20018590</v>
+      </c>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I39" s="12"/>
+      <c r="J39" s="12">
+        <v>6952101001</v>
+      </c>
+      <c r="K39" s="13">
+        <v>43990</v>
+      </c>
+      <c r="L39" s="14">
+        <v>0.65570601851851851</v>
+      </c>
+      <c r="M39" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N39" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4"/>
+      <c r="S39" s="4"/>
+      <c r="T39" s="4"/>
+      <c r="U39" s="4"/>
+      <c r="V39" s="4"/>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" s="9">
+        <v>211</v>
+      </c>
+      <c r="C40" s="9">
+        <v>12312274</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E40" s="9">
+        <v>104</v>
+      </c>
+      <c r="F40" s="9">
+        <v>20018590</v>
+      </c>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9">
+        <v>6952101001</v>
+      </c>
+      <c r="K40" s="10">
+        <v>43990</v>
+      </c>
+      <c r="L40" s="11">
+        <v>0.65725694444444438</v>
+      </c>
+      <c r="M40" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="N40" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="O40" s="4"/>
+      <c r="P40" s="4"/>
+      <c r="Q40" s="4"/>
+      <c r="R40" s="4"/>
+      <c r="S40" s="4"/>
+      <c r="T40" s="4"/>
+      <c r="U40" s="4"/>
+      <c r="V40" s="4"/>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" s="12">
+        <v>211</v>
+      </c>
+      <c r="C41" s="12">
+        <v>19130584</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E41" s="12">
+        <v>104</v>
+      </c>
+      <c r="F41" s="12">
+        <v>20018591</v>
+      </c>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12">
+        <v>6952101001</v>
+      </c>
+      <c r="K41" s="13">
+        <v>43990</v>
+      </c>
+      <c r="L41" s="14">
+        <v>0.65640046296296295</v>
+      </c>
+      <c r="M41" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N41" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4"/>
+      <c r="S41" s="4"/>
+      <c r="T41" s="4"/>
+      <c r="U41" s="4"/>
+      <c r="V41" s="4"/>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A42" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" s="9">
+        <v>211</v>
+      </c>
+      <c r="C42" s="9">
+        <v>12312274</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E42" s="9">
+        <v>104</v>
+      </c>
+      <c r="F42" s="9">
+        <v>20018591</v>
+      </c>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9">
+        <v>6952101001</v>
+      </c>
+      <c r="K42" s="10">
+        <v>43990</v>
+      </c>
+      <c r="L42" s="11">
+        <v>0.65795138888888893</v>
+      </c>
+      <c r="M42" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="N42" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="O42" s="4"/>
+      <c r="P42" s="4"/>
+      <c r="Q42" s="4"/>
+      <c r="R42" s="4"/>
+      <c r="S42" s="4"/>
+      <c r="T42" s="4"/>
+      <c r="U42" s="4"/>
+      <c r="V42" s="4"/>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="12">
+        <v>211</v>
+      </c>
+      <c r="C43" s="12">
+        <v>19130584</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E43" s="12">
+        <v>104</v>
+      </c>
+      <c r="F43" s="12">
+        <v>20018592</v>
+      </c>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I43" s="12"/>
+      <c r="J43" s="12">
+        <v>6952101001</v>
+      </c>
+      <c r="K43" s="13">
+        <v>43990</v>
+      </c>
+      <c r="L43" s="14">
+        <v>0.65709490740740739</v>
+      </c>
+      <c r="M43" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N43" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="4"/>
+      <c r="S43" s="4"/>
+      <c r="T43" s="4"/>
+      <c r="U43" s="4"/>
+      <c r="V43" s="4"/>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A44" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B44" s="9">
+        <v>211</v>
+      </c>
+      <c r="C44" s="9">
+        <v>12312274</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E44" s="9">
+        <v>104</v>
+      </c>
+      <c r="F44" s="9">
+        <v>20018592</v>
+      </c>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9">
+        <v>6952101001</v>
+      </c>
+      <c r="K44" s="10">
+        <v>43990</v>
+      </c>
+      <c r="L44" s="11">
+        <v>0.65864583333333326</v>
+      </c>
+      <c r="M44" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="N44" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="O44" s="4"/>
+      <c r="P44" s="4"/>
+      <c r="Q44" s="4"/>
+      <c r="R44" s="4"/>
+      <c r="S44" s="4"/>
+      <c r="T44" s="4"/>
+      <c r="U44" s="4"/>
+      <c r="V44" s="4"/>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A45" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" s="12">
+        <v>211</v>
+      </c>
+      <c r="C45" s="12">
+        <v>19130584</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="12">
+        <v>104</v>
+      </c>
+      <c r="F45" s="12">
+        <v>20018593</v>
+      </c>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I45" s="12"/>
+      <c r="J45" s="12">
+        <v>6952101001</v>
+      </c>
+      <c r="K45" s="13">
+        <v>43990</v>
+      </c>
+      <c r="L45" s="14">
+        <v>0.65778935185185183</v>
+      </c>
+      <c r="M45" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N45" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O45" s="4"/>
+      <c r="P45" s="4"/>
+      <c r="Q45" s="4"/>
+      <c r="R45" s="4"/>
+      <c r="S45" s="4"/>
+      <c r="T45" s="4"/>
+      <c r="U45" s="4"/>
+      <c r="V45" s="4"/>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A46" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" s="9">
+        <v>211</v>
+      </c>
+      <c r="C46" s="9">
+        <v>12312274</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E46" s="9">
+        <v>104</v>
+      </c>
+      <c r="F46" s="9">
+        <v>20018593</v>
+      </c>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9">
+        <v>6952101001</v>
+      </c>
+      <c r="K46" s="10">
+        <v>43990</v>
+      </c>
+      <c r="L46" s="11">
+        <v>0.65934027777777782</v>
+      </c>
+      <c r="M46" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="N46" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="O46" s="4"/>
+      <c r="P46" s="4"/>
+      <c r="Q46" s="4"/>
+      <c r="R46" s="4"/>
+      <c r="S46" s="4"/>
+      <c r="T46" s="4"/>
+      <c r="U46" s="4"/>
+      <c r="V46" s="4"/>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A47" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B47" s="12">
+        <v>211</v>
+      </c>
+      <c r="C47" s="12">
+        <v>19130584</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E47" s="12">
+        <v>104</v>
+      </c>
+      <c r="F47" s="12">
+        <v>20018594</v>
+      </c>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I47" s="12"/>
+      <c r="J47" s="12">
+        <v>6952101001</v>
+      </c>
+      <c r="K47" s="13">
+        <v>43990</v>
+      </c>
+      <c r="L47" s="14">
+        <v>0.65848379629629628</v>
+      </c>
+      <c r="M47" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N47" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O47" s="4"/>
+      <c r="P47" s="4"/>
+      <c r="Q47" s="4"/>
+      <c r="R47" s="4"/>
+      <c r="S47" s="4"/>
+      <c r="T47" s="4"/>
+      <c r="U47" s="4"/>
+      <c r="V47" s="4"/>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B48" s="9">
+        <v>211</v>
+      </c>
+      <c r="C48" s="9">
+        <v>12312274</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E48" s="9">
+        <v>104</v>
+      </c>
+      <c r="F48" s="9">
+        <v>20018594</v>
+      </c>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9">
+        <v>6952101001</v>
+      </c>
+      <c r="K48" s="10">
+        <v>43990</v>
+      </c>
+      <c r="L48" s="11">
+        <v>0.66003472222222226</v>
+      </c>
+      <c r="M48" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="N48" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="O48" s="4"/>
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4"/>
+      <c r="R48" s="4"/>
+      <c r="S48" s="4"/>
+      <c r="T48" s="4"/>
+      <c r="U48" s="4"/>
+      <c r="V48" s="4"/>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A49" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B49" s="12">
+        <v>211</v>
+      </c>
+      <c r="C49" s="12">
+        <v>15283381</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E49" s="12">
+        <v>110</v>
+      </c>
+      <c r="F49" s="12">
+        <v>20018595</v>
+      </c>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="I49" s="12"/>
+      <c r="J49" s="12">
+        <v>6952101001</v>
+      </c>
+      <c r="K49" s="13">
+        <v>43990</v>
+      </c>
+      <c r="L49" s="14">
+        <v>0.6607291666666667</v>
+      </c>
+      <c r="M49" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="N49" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="4"/>
+      <c r="S49" s="4"/>
+      <c r="T49" s="4"/>
+      <c r="U49" s="4"/>
+      <c r="V49" s="4"/>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A50" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B50" s="9">
+        <v>211</v>
+      </c>
+      <c r="C50" s="9">
+        <v>19130584</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E50" s="9">
+        <v>110</v>
+      </c>
+      <c r="F50" s="9">
+        <v>20018595</v>
+      </c>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9">
+        <v>6952101001</v>
+      </c>
+      <c r="K50" s="10">
+        <v>43990</v>
+      </c>
+      <c r="L50" s="11">
+        <v>0.66142361111111114</v>
+      </c>
+      <c r="M50" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="N50" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+      <c r="Q50" s="4"/>
+      <c r="R50" s="4"/>
+      <c r="S50" s="4"/>
+      <c r="T50" s="4"/>
+      <c r="U50" s="4"/>
+      <c r="V50" s="4"/>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A51" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B51" s="12">
+        <v>211</v>
+      </c>
+      <c r="C51" s="12">
+        <v>19130584</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E51" s="12">
+        <v>104</v>
+      </c>
+      <c r="F51" s="12">
+        <v>20018595</v>
+      </c>
+      <c r="G51" s="12"/>
+      <c r="H51" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I51" s="12"/>
+      <c r="J51" s="12">
+        <v>6952101001</v>
+      </c>
+      <c r="K51" s="13">
+        <v>43990</v>
+      </c>
+      <c r="L51" s="14">
+        <v>0.66211805555555558</v>
+      </c>
+      <c r="M51" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="N51" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O51" s="4"/>
+      <c r="P51" s="4"/>
+      <c r="Q51" s="4"/>
+      <c r="R51" s="4"/>
+      <c r="S51" s="4"/>
+      <c r="T51" s="4"/>
+      <c r="U51" s="4"/>
+      <c r="V51" s="4"/>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A52" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B52" s="9">
+        <v>211</v>
+      </c>
+      <c r="C52" s="9">
+        <v>19130584</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E52" s="9">
+        <v>104</v>
+      </c>
+      <c r="F52" s="9">
+        <v>20018595</v>
+      </c>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I52" s="9"/>
+      <c r="J52" s="9">
+        <v>6952101001</v>
+      </c>
+      <c r="K52" s="10">
+        <v>43990</v>
+      </c>
+      <c r="L52" s="11">
+        <v>0.66281250000000003</v>
+      </c>
+      <c r="M52" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="N52" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="O52" s="4"/>
+      <c r="P52" s="4"/>
+      <c r="Q52" s="4"/>
+      <c r="R52" s="4"/>
+      <c r="S52" s="4"/>
+      <c r="T52" s="4"/>
+      <c r="U52" s="4"/>
+      <c r="V52" s="4"/>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A53" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53" s="12">
+        <v>211</v>
+      </c>
+      <c r="C53" s="12">
+        <v>12312274</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E53" s="12">
+        <v>104</v>
+      </c>
+      <c r="F53" s="12">
+        <v>20018595</v>
+      </c>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I53" s="12"/>
+      <c r="J53" s="12">
+        <v>6952101001</v>
+      </c>
+      <c r="K53" s="13">
+        <v>43990</v>
+      </c>
+      <c r="L53" s="14">
+        <v>0.66350694444444447</v>
+      </c>
+      <c r="M53" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N53" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="O53" s="4"/>
+      <c r="P53" s="4"/>
+      <c r="Q53" s="4"/>
+      <c r="R53" s="4"/>
+      <c r="S53" s="4"/>
+      <c r="T53" s="4"/>
+      <c r="U53" s="4"/>
+      <c r="V53" s="4"/>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A54" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54" s="9">
+        <v>211</v>
+      </c>
+      <c r="C54" s="9">
+        <v>19130584</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E54" s="9">
+        <v>104</v>
+      </c>
+      <c r="F54" s="9">
+        <v>20018596</v>
+      </c>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9">
+        <v>6952101001</v>
+      </c>
+      <c r="K54" s="10">
+        <v>43990</v>
+      </c>
+      <c r="L54" s="11">
+        <v>0.66403935185185181</v>
+      </c>
+      <c r="M54" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="N54" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="O54" s="4"/>
+      <c r="P54" s="4"/>
+      <c r="Q54" s="4"/>
+      <c r="R54" s="4"/>
+      <c r="S54" s="4"/>
+      <c r="T54" s="4"/>
+      <c r="U54" s="4"/>
+      <c r="V54" s="4"/>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A55" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" s="12">
+        <v>211</v>
+      </c>
+      <c r="C55" s="12">
+        <v>12312274</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E55" s="12">
+        <v>104</v>
+      </c>
+      <c r="F55" s="12">
+        <v>20018596</v>
+      </c>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I55" s="12"/>
+      <c r="J55" s="12">
+        <v>6952101001</v>
+      </c>
+      <c r="K55" s="13">
+        <v>43990</v>
+      </c>
+      <c r="L55" s="14">
+        <v>0.66489583333333335</v>
+      </c>
+      <c r="M55" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="N55" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="O55" s="4"/>
+      <c r="P55" s="4"/>
+      <c r="Q55" s="4"/>
+      <c r="R55" s="4"/>
+      <c r="S55" s="4"/>
+      <c r="T55" s="4"/>
+      <c r="U55" s="4"/>
+      <c r="V55" s="4"/>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A56" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B56" s="9">
+        <v>211</v>
+      </c>
+      <c r="C56" s="9">
+        <v>12312274</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E56" s="9">
+        <v>104</v>
+      </c>
+      <c r="F56" s="9">
+        <v>20018596</v>
+      </c>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9">
+        <v>6952101001</v>
+      </c>
+      <c r="K56" s="10">
+        <v>43990</v>
+      </c>
+      <c r="L56" s="11">
+        <v>0.66559027777777779</v>
+      </c>
+      <c r="M56" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="N56" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="O56" s="4"/>
+      <c r="P56" s="4"/>
+      <c r="Q56" s="4"/>
+      <c r="R56" s="4"/>
+      <c r="S56" s="4"/>
+      <c r="T56" s="4"/>
+      <c r="U56" s="4"/>
+      <c r="V56" s="4"/>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A57" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" s="12">
+        <v>211</v>
+      </c>
+      <c r="C57" s="12">
+        <v>19130584</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E57" s="12">
+        <v>104</v>
+      </c>
+      <c r="F57" s="12">
+        <v>20018597</v>
+      </c>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I57" s="12"/>
+      <c r="J57" s="12">
+        <v>6952101001</v>
+      </c>
+      <c r="K57" s="13">
+        <v>43990</v>
+      </c>
+      <c r="L57" s="14">
+        <v>0.66612268518518525</v>
+      </c>
+      <c r="M57" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N57" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O57" s="4"/>
+      <c r="P57" s="4"/>
+      <c r="Q57" s="4"/>
+      <c r="R57" s="4"/>
+      <c r="S57" s="4"/>
+      <c r="T57" s="4"/>
+      <c r="U57" s="4"/>
+      <c r="V57" s="4"/>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A58" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B58" s="9">
+        <v>211</v>
+      </c>
+      <c r="C58" s="9">
+        <v>12312274</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E58" s="9">
+        <v>104</v>
+      </c>
+      <c r="F58" s="9">
+        <v>20018597</v>
+      </c>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I58" s="9"/>
+      <c r="J58" s="9">
+        <v>6952101001</v>
+      </c>
+      <c r="K58" s="10">
+        <v>43990</v>
+      </c>
+      <c r="L58" s="11">
+        <v>0.66697916666666668</v>
+      </c>
+      <c r="M58" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="N58" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="O58" s="4"/>
+      <c r="P58" s="4"/>
+      <c r="Q58" s="4"/>
+      <c r="R58" s="4"/>
+      <c r="S58" s="4"/>
+      <c r="T58" s="4"/>
+      <c r="U58" s="4"/>
+      <c r="V58" s="4"/>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A59" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59" s="12">
+        <v>211</v>
+      </c>
+      <c r="C59" s="12">
+        <v>12312274</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E59" s="12">
+        <v>104</v>
+      </c>
+      <c r="F59" s="12">
+        <v>20018597</v>
+      </c>
+      <c r="G59" s="12"/>
+      <c r="H59" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I59" s="12"/>
+      <c r="J59" s="12">
+        <v>6952101001</v>
+      </c>
+      <c r="K59" s="13">
+        <v>43990</v>
+      </c>
+      <c r="L59" s="14">
+        <v>0.66767361111111112</v>
+      </c>
+      <c r="M59" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N59" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="O59" s="4"/>
+      <c r="P59" s="4"/>
+      <c r="Q59" s="4"/>
+      <c r="R59" s="4"/>
+      <c r="S59" s="4"/>
+      <c r="T59" s="4"/>
+      <c r="U59" s="4"/>
+      <c r="V59" s="4"/>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A60" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60" s="9">
+        <v>211</v>
+      </c>
+      <c r="C60" s="9">
+        <v>19130584</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E60" s="9">
+        <v>104</v>
+      </c>
+      <c r="F60" s="9">
+        <v>20018598</v>
+      </c>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9">
+        <v>6952101001</v>
+      </c>
+      <c r="K60" s="10">
+        <v>43990</v>
+      </c>
+      <c r="L60" s="11">
+        <v>0.66820601851851846</v>
+      </c>
+      <c r="M60" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="N60" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="O60" s="4"/>
+      <c r="P60" s="4"/>
+      <c r="Q60" s="4"/>
+      <c r="R60" s="4"/>
+      <c r="S60" s="4"/>
+      <c r="T60" s="4"/>
+      <c r="U60" s="4"/>
+      <c r="V60" s="4"/>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A61" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61" s="12">
+        <v>211</v>
+      </c>
+      <c r="C61" s="12">
+        <v>12312274</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E61" s="12">
+        <v>104</v>
+      </c>
+      <c r="F61" s="12">
+        <v>20018598</v>
+      </c>
+      <c r="G61" s="12"/>
+      <c r="H61" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I61" s="12"/>
+      <c r="J61" s="12">
+        <v>6952101001</v>
+      </c>
+      <c r="K61" s="13">
+        <v>43990</v>
+      </c>
+      <c r="L61" s="14">
+        <v>0.6690625</v>
+      </c>
+      <c r="M61" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N61" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="O61" s="4"/>
+      <c r="P61" s="4"/>
+      <c r="Q61" s="4"/>
+      <c r="R61" s="4"/>
+      <c r="S61" s="4"/>
+      <c r="T61" s="4"/>
+      <c r="U61" s="4"/>
+      <c r="V61" s="4"/>
+    </row>
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A62" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62" s="9">
+        <v>211</v>
+      </c>
+      <c r="C62" s="9">
+        <v>19130584</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E62" s="9">
+        <v>104</v>
+      </c>
+      <c r="F62" s="9">
+        <v>20018599</v>
+      </c>
+      <c r="G62" s="9"/>
+      <c r="H62" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I62" s="9"/>
+      <c r="J62" s="9">
+        <v>6952101001</v>
+      </c>
+      <c r="K62" s="10">
+        <v>43990</v>
+      </c>
+      <c r="L62" s="11">
+        <v>0.66820601851851846</v>
+      </c>
+      <c r="M62" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="N62" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="O62" s="4"/>
+      <c r="P62" s="4"/>
+      <c r="Q62" s="4"/>
+      <c r="R62" s="4"/>
+      <c r="S62" s="4"/>
+      <c r="T62" s="4"/>
+      <c r="U62" s="4"/>
+      <c r="V62" s="4"/>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A63" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" s="18">
+        <v>211</v>
+      </c>
+      <c r="C63" s="18">
+        <v>12312274</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E63" s="18">
+        <v>104</v>
+      </c>
+      <c r="F63" s="18">
+        <v>20018599</v>
+      </c>
+      <c r="G63" s="18"/>
+      <c r="H63" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I63" s="18"/>
+      <c r="J63" s="18">
+        <v>6952101001</v>
+      </c>
+      <c r="K63" s="19">
+        <v>43990</v>
+      </c>
+      <c r="L63" s="20">
+        <v>0.6690625</v>
+      </c>
+      <c r="M63" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="N63" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="O63" s="4"/>
+      <c r="P63" s="4"/>
+      <c r="Q63" s="4"/>
+      <c r="R63" s="4"/>
+      <c r="S63" s="4"/>
+      <c r="T63" s="4"/>
+      <c r="U63" s="4"/>
+      <c r="V63" s="4"/>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>200</v>
+      </c>
+      <c r="C64">
+        <v>14138562</v>
+      </c>
+      <c r="D64" t="s">
+        <v>64</v>
+      </c>
+      <c r="E64">
+        <v>110</v>
+      </c>
+      <c r="F64">
+        <v>20102318</v>
+      </c>
+      <c r="H64" t="s">
+        <v>55</v>
+      </c>
+      <c r="J64">
+        <v>6541901001</v>
+      </c>
+      <c r="K64" s="5">
+        <v>44046</v>
+      </c>
+      <c r="L64" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="M64" t="s">
+        <v>52</v>
+      </c>
+      <c r="N64" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>200</v>
+      </c>
+      <c r="C65">
+        <v>15283381</v>
+      </c>
+      <c r="D65" t="s">
+        <v>65</v>
+      </c>
+      <c r="E65">
+        <v>110</v>
+      </c>
+      <c r="F65">
+        <v>20102318</v>
+      </c>
+      <c r="H65" t="s">
+        <v>48</v>
+      </c>
+      <c r="J65">
+        <v>6541901001</v>
+      </c>
+      <c r="K65" s="5">
+        <v>44046</v>
+      </c>
+      <c r="L65" s="6">
+        <v>0.41736111111111113</v>
+      </c>
+      <c r="M65" t="s">
+        <v>52</v>
+      </c>
+      <c r="N65" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>63</v>
+      </c>
+      <c r="B66">
+        <v>200</v>
+      </c>
+      <c r="C66">
+        <v>14138562</v>
+      </c>
+      <c r="D66" t="s">
+        <v>64</v>
+      </c>
+      <c r="E66">
+        <v>110</v>
+      </c>
+      <c r="F66">
+        <v>20102319</v>
+      </c>
+      <c r="H66" t="s">
+        <v>55</v>
+      </c>
+      <c r="J66">
+        <v>6541901001</v>
+      </c>
+      <c r="K66" s="5">
+        <v>44046</v>
+      </c>
+      <c r="L66" s="6">
+        <v>0.41805555555555557</v>
+      </c>
+      <c r="M66" t="s">
+        <v>52</v>
+      </c>
+      <c r="N66" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>63</v>
+      </c>
+      <c r="B67">
+        <v>200</v>
+      </c>
+      <c r="C67">
+        <v>15283381</v>
+      </c>
+      <c r="D67" t="s">
+        <v>65</v>
+      </c>
+      <c r="E67">
+        <v>110</v>
+      </c>
+      <c r="F67">
+        <v>20102319</v>
+      </c>
+      <c r="H67" t="s">
+        <v>48</v>
+      </c>
+      <c r="J67">
+        <v>6541901001</v>
+      </c>
+      <c r="K67" s="5">
+        <v>44046</v>
+      </c>
+      <c r="L67" s="6">
+        <v>0.41875000000000001</v>
+      </c>
+      <c r="M67" t="s">
+        <v>52</v>
+      </c>
+      <c r="N67" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>63</v>
+      </c>
+      <c r="B68">
+        <v>200</v>
+      </c>
+      <c r="C68">
+        <v>14138562</v>
+      </c>
+      <c r="D68" t="s">
+        <v>64</v>
+      </c>
+      <c r="E68">
+        <v>110</v>
+      </c>
+      <c r="F68">
+        <v>20102320</v>
+      </c>
+      <c r="H68" t="s">
+        <v>55</v>
+      </c>
+      <c r="J68">
+        <v>6541901001</v>
+      </c>
+      <c r="K68" s="5">
+        <v>44046</v>
+      </c>
+      <c r="L68" s="6">
+        <v>0.41944444444444401</v>
+      </c>
+      <c r="M68" t="s">
+        <v>52</v>
+      </c>
+      <c r="N68" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>63</v>
+      </c>
+      <c r="B69">
+        <v>200</v>
+      </c>
+      <c r="C69">
+        <v>15283381</v>
+      </c>
+      <c r="D69" t="s">
+        <v>65</v>
+      </c>
+      <c r="E69">
+        <v>110</v>
+      </c>
+      <c r="F69">
+        <v>20102320</v>
+      </c>
+      <c r="H69" t="s">
+        <v>48</v>
+      </c>
+      <c r="J69">
+        <v>6541901001</v>
+      </c>
+      <c r="K69" s="5">
+        <v>44046</v>
+      </c>
+      <c r="L69" s="6">
+        <v>0.42013888888888901</v>
+      </c>
+      <c r="M69" t="s">
+        <v>52</v>
+      </c>
+      <c r="N69" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>63</v>
+      </c>
+      <c r="B70">
+        <v>200</v>
+      </c>
+      <c r="C70">
+        <v>14138562</v>
+      </c>
+      <c r="D70" t="s">
+        <v>64</v>
+      </c>
+      <c r="E70">
+        <v>110</v>
+      </c>
+      <c r="F70">
+        <v>20102321</v>
+      </c>
+      <c r="H70" t="s">
+        <v>55</v>
+      </c>
+      <c r="J70">
+        <v>6541901001</v>
+      </c>
+      <c r="K70" s="5">
+        <v>44046</v>
+      </c>
+      <c r="L70" s="6">
+        <v>0.420833333333333</v>
+      </c>
+      <c r="M70" t="s">
+        <v>52</v>
+      </c>
+      <c r="N70" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>63</v>
+      </c>
+      <c r="B71">
+        <v>200</v>
+      </c>
+      <c r="C71">
+        <v>15283381</v>
+      </c>
+      <c r="D71" t="s">
+        <v>65</v>
+      </c>
+      <c r="E71">
+        <v>110</v>
+      </c>
+      <c r="F71">
+        <v>20102321</v>
+      </c>
+      <c r="H71" t="s">
+        <v>48</v>
+      </c>
+      <c r="J71">
+        <v>6541901001</v>
+      </c>
+      <c r="K71" s="5">
+        <v>44046</v>
+      </c>
+      <c r="L71" s="6">
+        <v>0.421527777777778</v>
+      </c>
+      <c r="M71" t="s">
+        <v>52</v>
+      </c>
+      <c r="N71" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>63</v>
+      </c>
+      <c r="B72">
+        <v>200</v>
+      </c>
+      <c r="C72">
+        <v>14138562</v>
+      </c>
+      <c r="D72" t="s">
+        <v>64</v>
+      </c>
+      <c r="E72">
+        <v>110</v>
+      </c>
+      <c r="F72">
+        <v>20102322</v>
+      </c>
+      <c r="H72" t="s">
+        <v>55</v>
+      </c>
+      <c r="J72">
+        <v>6541901001</v>
+      </c>
+      <c r="K72" s="5">
+        <v>44046</v>
+      </c>
+      <c r="L72" s="6">
+        <v>0.422222222222222</v>
+      </c>
+      <c r="M72" t="s">
+        <v>52</v>
+      </c>
+      <c r="N72" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>63</v>
+      </c>
+      <c r="B73">
+        <v>200</v>
+      </c>
+      <c r="C73">
+        <v>15283381</v>
+      </c>
+      <c r="D73" t="s">
+        <v>65</v>
+      </c>
+      <c r="E73">
+        <v>110</v>
+      </c>
+      <c r="F73">
+        <v>20102322</v>
+      </c>
+      <c r="H73" t="s">
+        <v>48</v>
+      </c>
+      <c r="J73">
+        <v>6541901001</v>
+      </c>
+      <c r="K73" s="5">
+        <v>44046</v>
+      </c>
+      <c r="L73" s="6">
+        <v>0.422916666666667</v>
+      </c>
+      <c r="M73" t="s">
+        <v>52</v>
+      </c>
+      <c r="N73" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>63</v>
+      </c>
+      <c r="B74">
+        <v>200</v>
+      </c>
+      <c r="C74">
+        <v>14138562</v>
+      </c>
+      <c r="D74" t="s">
+        <v>64</v>
+      </c>
+      <c r="E74">
+        <v>110</v>
+      </c>
+      <c r="F74">
+        <v>20102323</v>
+      </c>
+      <c r="H74" t="s">
+        <v>55</v>
+      </c>
+      <c r="J74">
+        <v>6541901001</v>
+      </c>
+      <c r="K74" s="5">
+        <v>44046</v>
+      </c>
+      <c r="L74" s="6">
+        <v>0.42361111111111099</v>
+      </c>
+      <c r="M74" t="s">
+        <v>52</v>
+      </c>
+      <c r="N74" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>63</v>
+      </c>
+      <c r="B75">
+        <v>200</v>
+      </c>
+      <c r="C75">
+        <v>15283381</v>
+      </c>
+      <c r="D75" t="s">
+        <v>65</v>
+      </c>
+      <c r="E75">
+        <v>110</v>
+      </c>
+      <c r="F75">
+        <v>20102323</v>
+      </c>
+      <c r="H75" t="s">
+        <v>48</v>
+      </c>
+      <c r="J75">
+        <v>6541901001</v>
+      </c>
+      <c r="K75" s="5">
+        <v>44046</v>
+      </c>
+      <c r="L75" s="6">
+        <v>0.42430555555555599</v>
+      </c>
+      <c r="M75" t="s">
+        <v>52</v>
+      </c>
+      <c r="N75" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>63</v>
+      </c>
+      <c r="B76">
+        <v>200</v>
+      </c>
+      <c r="C76">
+        <v>14138562</v>
+      </c>
+      <c r="D76" t="s">
+        <v>64</v>
+      </c>
+      <c r="E76">
+        <v>110</v>
+      </c>
+      <c r="F76">
+        <v>20102324</v>
+      </c>
+      <c r="H76" t="s">
+        <v>55</v>
+      </c>
+      <c r="J76">
+        <v>6541901001</v>
+      </c>
+      <c r="K76" s="5">
+        <v>44046</v>
+      </c>
+      <c r="L76" s="6">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="M76" t="s">
+        <v>52</v>
+      </c>
+      <c r="N76" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>63</v>
+      </c>
+      <c r="B77">
+        <v>200</v>
+      </c>
+      <c r="C77">
+        <v>15283381</v>
+      </c>
+      <c r="D77" t="s">
+        <v>65</v>
+      </c>
+      <c r="E77">
+        <v>110</v>
+      </c>
+      <c r="F77">
+        <v>20102324</v>
+      </c>
+      <c r="H77" t="s">
+        <v>48</v>
+      </c>
+      <c r="J77">
+        <v>6541901001</v>
+      </c>
+      <c r="K77" s="5">
+        <v>44046</v>
+      </c>
+      <c r="L77" s="6">
+        <v>0.42569444444444399</v>
+      </c>
+      <c r="M77" t="s">
+        <v>52</v>
+      </c>
+      <c r="N77" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>63</v>
+      </c>
+      <c r="B78">
+        <v>200</v>
+      </c>
+      <c r="C78">
+        <v>14138562</v>
+      </c>
+      <c r="D78" t="s">
+        <v>64</v>
+      </c>
+      <c r="E78">
+        <v>110</v>
+      </c>
+      <c r="F78">
+        <v>20102325</v>
+      </c>
+      <c r="H78" t="s">
+        <v>55</v>
+      </c>
+      <c r="J78">
+        <v>6541901001</v>
+      </c>
+      <c r="K78" s="5">
+        <v>44046</v>
+      </c>
+      <c r="L78" s="6">
+        <v>0.42638888888888898</v>
+      </c>
+      <c r="M78" t="s">
+        <v>52</v>
+      </c>
+      <c r="N78" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>63</v>
+      </c>
+      <c r="B79">
+        <v>200</v>
+      </c>
+      <c r="C79">
+        <v>15283381</v>
+      </c>
+      <c r="D79" t="s">
+        <v>65</v>
+      </c>
+      <c r="E79">
+        <v>110</v>
+      </c>
+      <c r="F79">
+        <v>20102325</v>
+      </c>
+      <c r="H79" t="s">
+        <v>48</v>
+      </c>
+      <c r="J79">
+        <v>6541901001</v>
+      </c>
+      <c r="K79" s="5">
+        <v>44046</v>
+      </c>
+      <c r="L79" s="6">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="M79" t="s">
+        <v>52</v>
+      </c>
+      <c r="N79" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>62</v>
+      </c>
+      <c r="B80">
+        <v>211</v>
+      </c>
+      <c r="C80">
+        <v>19130584</v>
+      </c>
+      <c r="D80" t="s">
+        <v>64</v>
+      </c>
+      <c r="E80">
+        <v>110</v>
+      </c>
+      <c r="F80">
+        <v>20102326</v>
+      </c>
+      <c r="H80" t="s">
+        <v>55</v>
+      </c>
+      <c r="J80">
+        <v>6541901001</v>
+      </c>
+      <c r="K80" s="5">
+        <v>44046</v>
+      </c>
+      <c r="L80" s="6">
+        <v>0.42777777777777781</v>
+      </c>
+      <c r="M80" t="s">
+        <v>50</v>
+      </c>
+      <c r="N80" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>62</v>
+      </c>
+      <c r="B81">
+        <v>211</v>
+      </c>
+      <c r="C81">
+        <v>19130584</v>
+      </c>
+      <c r="D81" t="s">
+        <v>64</v>
+      </c>
+      <c r="E81">
+        <v>110</v>
+      </c>
+      <c r="F81">
+        <v>20102326</v>
+      </c>
+      <c r="H81" t="s">
+        <v>55</v>
+      </c>
+      <c r="J81">
+        <v>6541901001</v>
+      </c>
+      <c r="K81" s="5">
+        <v>44046</v>
+      </c>
+      <c r="L81" s="6">
+        <v>0.4284722222222222</v>
+      </c>
+      <c r="M81" t="s">
+        <v>50</v>
+      </c>
+      <c r="N81" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>62</v>
+      </c>
+      <c r="B82">
+        <v>211</v>
+      </c>
+      <c r="C82">
+        <v>19130584</v>
+      </c>
+      <c r="D82" t="s">
+        <v>64</v>
+      </c>
+      <c r="E82">
+        <v>110</v>
+      </c>
+      <c r="F82">
+        <v>20102326</v>
+      </c>
+      <c r="H82" t="s">
+        <v>55</v>
+      </c>
+      <c r="J82">
+        <v>6541901001</v>
+      </c>
+      <c r="K82" s="5">
+        <v>44046</v>
+      </c>
+      <c r="L82" s="6">
+        <v>0.42916666666666697</v>
+      </c>
+      <c r="M82" t="s">
+        <v>50</v>
+      </c>
+      <c r="N82" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>62</v>
+      </c>
+      <c r="B83">
+        <v>211</v>
+      </c>
+      <c r="C83">
+        <v>19130584</v>
+      </c>
+      <c r="D83" t="s">
+        <v>64</v>
+      </c>
+      <c r="E83">
+        <v>110</v>
+      </c>
+      <c r="F83">
+        <v>20102326</v>
+      </c>
+      <c r="H83" t="s">
+        <v>55</v>
+      </c>
+      <c r="J83">
+        <v>6541901001</v>
+      </c>
+      <c r="K83" s="5">
+        <v>44046</v>
+      </c>
+      <c r="L83" s="6">
+        <v>0.42986111111111103</v>
+      </c>
+      <c r="M83" t="s">
+        <v>50</v>
+      </c>
+      <c r="N83" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>63</v>
+      </c>
+      <c r="B84">
+        <v>200</v>
+      </c>
+      <c r="C84">
+        <v>14138562</v>
+      </c>
+      <c r="D84" t="s">
+        <v>64</v>
+      </c>
+      <c r="E84">
+        <v>110</v>
+      </c>
+      <c r="F84">
+        <v>20102326</v>
+      </c>
+      <c r="H84" t="s">
+        <v>55</v>
+      </c>
+      <c r="J84">
+        <v>6541901001</v>
+      </c>
+      <c r="K84" s="5">
+        <v>44046</v>
+      </c>
+      <c r="L84" s="6">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="M84" t="s">
+        <v>52</v>
+      </c>
+      <c r="N84" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>63</v>
+      </c>
+      <c r="B85">
+        <v>200</v>
+      </c>
+      <c r="C85">
+        <v>15283381</v>
+      </c>
+      <c r="D85" t="s">
+        <v>65</v>
+      </c>
+      <c r="E85">
+        <v>110</v>
+      </c>
+      <c r="F85">
+        <v>20102326</v>
+      </c>
+      <c r="H85" t="s">
+        <v>48</v>
+      </c>
+      <c r="J85">
+        <v>6541901001</v>
+      </c>
+      <c r="K85" s="5">
+        <v>44046</v>
+      </c>
+      <c r="L85" s="6">
+        <v>0.43124999999999997</v>
+      </c>
+      <c r="M85" t="s">
+        <v>52</v>
+      </c>
+      <c r="N85" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>63</v>
+      </c>
+      <c r="B86">
+        <v>200</v>
+      </c>
+      <c r="C86">
+        <v>14138562</v>
+      </c>
+      <c r="D86" t="s">
+        <v>64</v>
+      </c>
+      <c r="E86">
+        <v>110</v>
+      </c>
+      <c r="F86">
+        <v>20102327</v>
+      </c>
+      <c r="H86" t="s">
+        <v>55</v>
+      </c>
+      <c r="J86">
+        <v>6541901001</v>
+      </c>
+      <c r="K86" s="5">
+        <v>44046</v>
+      </c>
+      <c r="L86" s="6">
+        <v>0.43194444444444446</v>
+      </c>
+      <c r="M86" t="s">
+        <v>52</v>
+      </c>
+      <c r="N86" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>62</v>
+      </c>
+      <c r="B87">
+        <v>211</v>
+      </c>
+      <c r="C87">
+        <v>19130584</v>
+      </c>
+      <c r="D87" t="s">
+        <v>65</v>
+      </c>
+      <c r="E87">
+        <v>110</v>
+      </c>
+      <c r="F87">
+        <v>20102327</v>
+      </c>
+      <c r="H87" t="s">
+        <v>48</v>
+      </c>
+      <c r="J87">
+        <v>6541901001</v>
+      </c>
+      <c r="K87" s="5">
+        <v>44046</v>
+      </c>
+      <c r="L87" s="6">
+        <v>0.43263888888888885</v>
+      </c>
+      <c r="M87" t="s">
+        <v>50</v>
+      </c>
+      <c r="N87" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>63</v>
+      </c>
+      <c r="B88">
+        <v>200</v>
+      </c>
+      <c r="C88">
+        <v>19130584</v>
+      </c>
+      <c r="D88" t="s">
+        <v>65</v>
+      </c>
+      <c r="E88">
+        <v>110</v>
+      </c>
+      <c r="F88">
+        <v>20102327</v>
+      </c>
+      <c r="H88" t="s">
+        <v>48</v>
+      </c>
+      <c r="J88">
+        <v>6541901001</v>
+      </c>
+      <c r="K88" s="5">
+        <v>44046</v>
+      </c>
+      <c r="L88" s="6">
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="M88" t="s">
+        <v>52</v>
+      </c>
+      <c r="N88" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2269,21 +4733,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -2338,7 +4802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -2349,10 +4813,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="8"/>
+      <c r="B1" s="7"/>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>60</v>
       </c>
       <c r="D2" t="s">
@@ -2360,17 +4824,17 @@
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Filter that show true first passed approved products
</commit_message>
<xml_diff>
--- a/apps/dataset/Database.xlsx
+++ b/apps/dataset/Database.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="overview" sheetId="1" r:id="rId1"/>
     <sheet name="zz8" sheetId="2" r:id="rId2"/>
     <sheet name="zz9" sheetId="3" r:id="rId3"/>
     <sheet name="Exemplos necessários" sheetId="4" r:id="rId4"/>
+    <sheet name="Reprovados" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="68">
   <si>
     <t>Nome etapa</t>
   </si>
@@ -215,6 +216,12 @@
   </si>
   <si>
     <t>TXRAIL-USB-VALIDAÇÃO</t>
+  </si>
+  <si>
+    <t>Reprovados</t>
+  </si>
+  <si>
+    <t>Aprovados</t>
   </si>
 </sst>
 </file>
@@ -345,9 +352,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="21" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -360,6 +364,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -745,21 +752,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
     </row>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -891,30 +898,30 @@
       </c>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
-      <c r="W7" s="8"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="20"/>
+      <c r="V7" s="20"/>
+      <c r="W7" s="20"/>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -1049,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="C61" workbookViewId="0">
+      <selection activeCell="F78" activeCellId="21" sqref="F10 F11 F14 F15 F17 F31 F33 F39 F41 F43 F45 F48 F61 F62 F64 F66 F68 F70 F72 F74 F76 F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,30 +1081,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -2308,42 +2315,42 @@
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
+      <c r="A34" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="9">
-        <v>211</v>
-      </c>
-      <c r="C34" s="9">
+      <c r="B34" s="8">
+        <v>211</v>
+      </c>
+      <c r="C34" s="8">
         <v>19130584</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E34" s="9">
+      <c r="E34" s="8">
         <v>110</v>
       </c>
-      <c r="F34" s="9">
+      <c r="F34" s="8">
         <v>20018589</v>
       </c>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9" t="s">
+      <c r="G34" s="8"/>
+      <c r="H34" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="I34" s="9"/>
-      <c r="J34" s="9">
-        <v>6952101001</v>
-      </c>
-      <c r="K34" s="10">
+      <c r="I34" s="8"/>
+      <c r="J34" s="8">
+        <v>6952101001</v>
+      </c>
+      <c r="K34" s="9">
         <v>43990</v>
       </c>
-      <c r="L34" s="11">
+      <c r="L34" s="10">
         <v>0.53003472222222225</v>
       </c>
-      <c r="M34" s="9" t="s">
+      <c r="M34" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="N34" s="9" t="s">
+      <c r="N34" s="8" t="s">
         <v>51</v>
       </c>
       <c r="O34" s="4"/>
@@ -2356,42 +2363,42 @@
       <c r="V34" s="4"/>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="12">
-        <v>211</v>
-      </c>
-      <c r="C35" s="12">
+      <c r="B35" s="11">
+        <v>211</v>
+      </c>
+      <c r="C35" s="11">
         <v>19130584</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E35" s="12">
+      <c r="E35" s="11">
         <v>110</v>
       </c>
-      <c r="F35" s="12">
+      <c r="F35" s="11">
         <v>20018589</v>
       </c>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12" t="s">
+      <c r="G35" s="11"/>
+      <c r="H35" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12">
-        <v>6952101001</v>
-      </c>
-      <c r="K35" s="13">
+      <c r="I35" s="11"/>
+      <c r="J35" s="11">
+        <v>6952101001</v>
+      </c>
+      <c r="K35" s="12">
         <v>43990</v>
       </c>
-      <c r="L35" s="14">
+      <c r="L35" s="13">
         <v>0.53070601851851851</v>
       </c>
-      <c r="M35" s="12" t="s">
+      <c r="M35" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="N35" s="12" t="s">
+      <c r="N35" s="11" t="s">
         <v>51</v>
       </c>
       <c r="O35" s="4"/>
@@ -2404,42 +2411,42 @@
       <c r="V35" s="4"/>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B36" s="9">
-        <v>211</v>
-      </c>
-      <c r="C36" s="9">
+      <c r="B36" s="8">
+        <v>211</v>
+      </c>
+      <c r="C36" s="8">
         <v>19130584</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E36" s="9">
-        <v>104</v>
-      </c>
-      <c r="F36" s="9">
+      <c r="E36" s="8">
+        <v>104</v>
+      </c>
+      <c r="F36" s="8">
         <v>20018589</v>
       </c>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9" t="s">
+      <c r="G36" s="8"/>
+      <c r="H36" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="I36" s="9"/>
-      <c r="J36" s="9">
-        <v>6952101001</v>
-      </c>
-      <c r="K36" s="10">
+      <c r="I36" s="8"/>
+      <c r="J36" s="8">
+        <v>6952101001</v>
+      </c>
+      <c r="K36" s="9">
         <v>43990</v>
       </c>
-      <c r="L36" s="11">
+      <c r="L36" s="10">
         <v>0.53070601851851851</v>
       </c>
-      <c r="M36" s="9" t="s">
+      <c r="M36" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="N36" s="9" t="s">
+      <c r="N36" s="8" t="s">
         <v>51</v>
       </c>
       <c r="O36" s="4"/>
@@ -2452,42 +2459,42 @@
       <c r="V36" s="4"/>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B37" s="12">
-        <v>211</v>
-      </c>
-      <c r="C37" s="12">
+      <c r="B37" s="11">
+        <v>211</v>
+      </c>
+      <c r="C37" s="11">
         <v>19130584</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E37" s="12">
-        <v>104</v>
-      </c>
-      <c r="F37" s="12">
+      <c r="E37" s="11">
+        <v>104</v>
+      </c>
+      <c r="F37" s="11">
         <v>20018589</v>
       </c>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12" t="s">
+      <c r="G37" s="11"/>
+      <c r="H37" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I37" s="12"/>
-      <c r="J37" s="12">
-        <v>6952101001</v>
-      </c>
-      <c r="K37" s="13">
+      <c r="I37" s="11"/>
+      <c r="J37" s="11">
+        <v>6952101001</v>
+      </c>
+      <c r="K37" s="12">
         <v>43990</v>
       </c>
-      <c r="L37" s="14">
+      <c r="L37" s="13">
         <v>0.53070601851851851</v>
       </c>
-      <c r="M37" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="N37" s="12" t="s">
+      <c r="M37" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="N37" s="11" t="s">
         <v>51</v>
       </c>
       <c r="O37" s="4"/>
@@ -2500,42 +2507,42 @@
       <c r="V37" s="4"/>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A38" s="16" t="s">
+      <c r="A38" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B38" s="9">
-        <v>211</v>
-      </c>
-      <c r="C38" s="9">
+      <c r="B38" s="8">
+        <v>211</v>
+      </c>
+      <c r="C38" s="8">
         <v>12312274</v>
       </c>
-      <c r="D38" s="9" t="s">
+      <c r="D38" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E38" s="9">
-        <v>104</v>
-      </c>
-      <c r="F38" s="9">
+      <c r="E38" s="8">
+        <v>104</v>
+      </c>
+      <c r="F38" s="8">
         <v>20018589</v>
       </c>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9" t="s">
+      <c r="G38" s="8"/>
+      <c r="H38" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="I38" s="9"/>
-      <c r="J38" s="9">
-        <v>6952101001</v>
-      </c>
-      <c r="K38" s="10">
+      <c r="I38" s="8"/>
+      <c r="J38" s="8">
+        <v>6952101001</v>
+      </c>
+      <c r="K38" s="9">
         <v>43990</v>
       </c>
-      <c r="L38" s="11">
+      <c r="L38" s="10">
         <v>0.64475694444444442</v>
       </c>
-      <c r="M38" s="9" t="s">
+      <c r="M38" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="N38" s="9" t="s">
+      <c r="N38" s="8" t="s">
         <v>56</v>
       </c>
       <c r="O38" s="4"/>
@@ -2548,42 +2555,42 @@
       <c r="V38" s="4"/>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A39" s="15" t="s">
+      <c r="A39" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B39" s="12">
-        <v>211</v>
-      </c>
-      <c r="C39" s="12">
+      <c r="B39" s="11">
+        <v>211</v>
+      </c>
+      <c r="C39" s="11">
         <v>19130584</v>
       </c>
-      <c r="D39" s="12" t="s">
+      <c r="D39" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E39" s="12">
-        <v>104</v>
-      </c>
-      <c r="F39" s="12">
+      <c r="E39" s="11">
+        <v>104</v>
+      </c>
+      <c r="F39" s="11">
         <v>20018590</v>
       </c>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12" t="s">
+      <c r="G39" s="11"/>
+      <c r="H39" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I39" s="12"/>
-      <c r="J39" s="12">
-        <v>6952101001</v>
-      </c>
-      <c r="K39" s="13">
+      <c r="I39" s="11"/>
+      <c r="J39" s="11">
+        <v>6952101001</v>
+      </c>
+      <c r="K39" s="12">
         <v>43990</v>
       </c>
-      <c r="L39" s="14">
+      <c r="L39" s="13">
         <v>0.65570601851851851</v>
       </c>
-      <c r="M39" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="N39" s="12" t="s">
+      <c r="M39" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="N39" s="11" t="s">
         <v>51</v>
       </c>
       <c r="O39" s="4"/>
@@ -2596,42 +2603,42 @@
       <c r="V39" s="4"/>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
+      <c r="A40" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="9">
-        <v>211</v>
-      </c>
-      <c r="C40" s="9">
+      <c r="B40" s="8">
+        <v>211</v>
+      </c>
+      <c r="C40" s="8">
         <v>12312274</v>
       </c>
-      <c r="D40" s="9" t="s">
+      <c r="D40" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E40" s="9">
-        <v>104</v>
-      </c>
-      <c r="F40" s="9">
+      <c r="E40" s="8">
+        <v>104</v>
+      </c>
+      <c r="F40" s="8">
         <v>20018590</v>
       </c>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9" t="s">
+      <c r="G40" s="8"/>
+      <c r="H40" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="I40" s="9"/>
-      <c r="J40" s="9">
-        <v>6952101001</v>
-      </c>
-      <c r="K40" s="10">
+      <c r="I40" s="8"/>
+      <c r="J40" s="8">
+        <v>6952101001</v>
+      </c>
+      <c r="K40" s="9">
         <v>43990</v>
       </c>
-      <c r="L40" s="11">
+      <c r="L40" s="10">
         <v>0.65725694444444438</v>
       </c>
-      <c r="M40" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="N40" s="9" t="s">
+      <c r="M40" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N40" s="8" t="s">
         <v>56</v>
       </c>
       <c r="O40" s="4"/>
@@ -2644,42 +2651,42 @@
       <c r="V40" s="4"/>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="12">
-        <v>211</v>
-      </c>
-      <c r="C41" s="12">
+      <c r="B41" s="11">
+        <v>211</v>
+      </c>
+      <c r="C41" s="11">
         <v>19130584</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D41" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E41" s="12">
-        <v>104</v>
-      </c>
-      <c r="F41" s="12">
+      <c r="E41" s="11">
+        <v>104</v>
+      </c>
+      <c r="F41" s="11">
         <v>20018591</v>
       </c>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12" t="s">
+      <c r="G41" s="11"/>
+      <c r="H41" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I41" s="12"/>
-      <c r="J41" s="12">
-        <v>6952101001</v>
-      </c>
-      <c r="K41" s="13">
+      <c r="I41" s="11"/>
+      <c r="J41" s="11">
+        <v>6952101001</v>
+      </c>
+      <c r="K41" s="12">
         <v>43990</v>
       </c>
-      <c r="L41" s="14">
+      <c r="L41" s="13">
         <v>0.65640046296296295</v>
       </c>
-      <c r="M41" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="N41" s="12" t="s">
+      <c r="M41" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="N41" s="11" t="s">
         <v>51</v>
       </c>
       <c r="O41" s="4"/>
@@ -2692,42 +2699,42 @@
       <c r="V41" s="4"/>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A42" s="16" t="s">
+      <c r="A42" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="9">
-        <v>211</v>
-      </c>
-      <c r="C42" s="9">
+      <c r="B42" s="8">
+        <v>211</v>
+      </c>
+      <c r="C42" s="8">
         <v>12312274</v>
       </c>
-      <c r="D42" s="9" t="s">
+      <c r="D42" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E42" s="9">
-        <v>104</v>
-      </c>
-      <c r="F42" s="9">
+      <c r="E42" s="8">
+        <v>104</v>
+      </c>
+      <c r="F42" s="8">
         <v>20018591</v>
       </c>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9" t="s">
+      <c r="G42" s="8"/>
+      <c r="H42" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="I42" s="9"/>
-      <c r="J42" s="9">
-        <v>6952101001</v>
-      </c>
-      <c r="K42" s="10">
+      <c r="I42" s="8"/>
+      <c r="J42" s="8">
+        <v>6952101001</v>
+      </c>
+      <c r="K42" s="9">
         <v>43990</v>
       </c>
-      <c r="L42" s="11">
+      <c r="L42" s="10">
         <v>0.65795138888888893</v>
       </c>
-      <c r="M42" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="N42" s="9" t="s">
+      <c r="M42" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N42" s="8" t="s">
         <v>56</v>
       </c>
       <c r="O42" s="4"/>
@@ -2740,42 +2747,42 @@
       <c r="V42" s="4"/>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A43" s="15" t="s">
+      <c r="A43" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B43" s="12">
-        <v>211</v>
-      </c>
-      <c r="C43" s="12">
+      <c r="B43" s="11">
+        <v>211</v>
+      </c>
+      <c r="C43" s="11">
         <v>19130584</v>
       </c>
-      <c r="D43" s="12" t="s">
+      <c r="D43" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E43" s="12">
-        <v>104</v>
-      </c>
-      <c r="F43" s="12">
+      <c r="E43" s="11">
+        <v>104</v>
+      </c>
+      <c r="F43" s="11">
         <v>20018592</v>
       </c>
-      <c r="G43" s="12"/>
-      <c r="H43" s="12" t="s">
+      <c r="G43" s="11"/>
+      <c r="H43" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I43" s="12"/>
-      <c r="J43" s="12">
-        <v>6952101001</v>
-      </c>
-      <c r="K43" s="13">
+      <c r="I43" s="11"/>
+      <c r="J43" s="11">
+        <v>6952101001</v>
+      </c>
+      <c r="K43" s="12">
         <v>43990</v>
       </c>
-      <c r="L43" s="14">
+      <c r="L43" s="13">
         <v>0.65709490740740739</v>
       </c>
-      <c r="M43" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="N43" s="12" t="s">
+      <c r="M43" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="N43" s="11" t="s">
         <v>51</v>
       </c>
       <c r="O43" s="4"/>
@@ -2788,42 +2795,42 @@
       <c r="V43" s="4"/>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A44" s="16" t="s">
+      <c r="A44" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B44" s="9">
-        <v>211</v>
-      </c>
-      <c r="C44" s="9">
+      <c r="B44" s="8">
+        <v>211</v>
+      </c>
+      <c r="C44" s="8">
         <v>12312274</v>
       </c>
-      <c r="D44" s="9" t="s">
+      <c r="D44" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E44" s="9">
-        <v>104</v>
-      </c>
-      <c r="F44" s="9">
+      <c r="E44" s="8">
+        <v>104</v>
+      </c>
+      <c r="F44" s="8">
         <v>20018592</v>
       </c>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9" t="s">
+      <c r="G44" s="8"/>
+      <c r="H44" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="I44" s="9"/>
-      <c r="J44" s="9">
-        <v>6952101001</v>
-      </c>
-      <c r="K44" s="10">
+      <c r="I44" s="8"/>
+      <c r="J44" s="8">
+        <v>6952101001</v>
+      </c>
+      <c r="K44" s="9">
         <v>43990</v>
       </c>
-      <c r="L44" s="11">
+      <c r="L44" s="10">
         <v>0.65864583333333326</v>
       </c>
-      <c r="M44" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="N44" s="9" t="s">
+      <c r="M44" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N44" s="8" t="s">
         <v>56</v>
       </c>
       <c r="O44" s="4"/>
@@ -2836,42 +2843,42 @@
       <c r="V44" s="4"/>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A45" s="15" t="s">
+      <c r="A45" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B45" s="12">
-        <v>211</v>
-      </c>
-      <c r="C45" s="12">
+      <c r="B45" s="11">
+        <v>211</v>
+      </c>
+      <c r="C45" s="11">
         <v>19130584</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D45" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E45" s="12">
-        <v>104</v>
-      </c>
-      <c r="F45" s="12">
+      <c r="E45" s="11">
+        <v>104</v>
+      </c>
+      <c r="F45" s="11">
         <v>20018593</v>
       </c>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12" t="s">
+      <c r="G45" s="11"/>
+      <c r="H45" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I45" s="12"/>
-      <c r="J45" s="12">
-        <v>6952101001</v>
-      </c>
-      <c r="K45" s="13">
+      <c r="I45" s="11"/>
+      <c r="J45" s="11">
+        <v>6952101001</v>
+      </c>
+      <c r="K45" s="12">
         <v>43990</v>
       </c>
-      <c r="L45" s="14">
+      <c r="L45" s="13">
         <v>0.65778935185185183</v>
       </c>
-      <c r="M45" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="N45" s="12" t="s">
+      <c r="M45" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="N45" s="11" t="s">
         <v>51</v>
       </c>
       <c r="O45" s="4"/>
@@ -2884,42 +2891,42 @@
       <c r="V45" s="4"/>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A46" s="16" t="s">
+      <c r="A46" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B46" s="9">
-        <v>211</v>
-      </c>
-      <c r="C46" s="9">
+      <c r="B46" s="8">
+        <v>211</v>
+      </c>
+      <c r="C46" s="8">
         <v>12312274</v>
       </c>
-      <c r="D46" s="9" t="s">
+      <c r="D46" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E46" s="9">
-        <v>104</v>
-      </c>
-      <c r="F46" s="9">
+      <c r="E46" s="8">
+        <v>104</v>
+      </c>
+      <c r="F46" s="8">
         <v>20018593</v>
       </c>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9" t="s">
+      <c r="G46" s="8"/>
+      <c r="H46" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9">
-        <v>6952101001</v>
-      </c>
-      <c r="K46" s="10">
+      <c r="I46" s="8"/>
+      <c r="J46" s="8">
+        <v>6952101001</v>
+      </c>
+      <c r="K46" s="9">
         <v>43990</v>
       </c>
-      <c r="L46" s="11">
+      <c r="L46" s="10">
         <v>0.65934027777777782</v>
       </c>
-      <c r="M46" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="N46" s="9" t="s">
+      <c r="M46" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N46" s="8" t="s">
         <v>56</v>
       </c>
       <c r="O46" s="4"/>
@@ -2932,42 +2939,42 @@
       <c r="V46" s="4"/>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B47" s="12">
-        <v>211</v>
-      </c>
-      <c r="C47" s="12">
+      <c r="B47" s="11">
+        <v>211</v>
+      </c>
+      <c r="C47" s="11">
         <v>19130584</v>
       </c>
-      <c r="D47" s="12" t="s">
+      <c r="D47" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E47" s="12">
-        <v>104</v>
-      </c>
-      <c r="F47" s="12">
+      <c r="E47" s="11">
+        <v>104</v>
+      </c>
+      <c r="F47" s="11">
         <v>20018594</v>
       </c>
-      <c r="G47" s="12"/>
-      <c r="H47" s="12" t="s">
+      <c r="G47" s="11"/>
+      <c r="H47" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I47" s="12"/>
-      <c r="J47" s="12">
-        <v>6952101001</v>
-      </c>
-      <c r="K47" s="13">
+      <c r="I47" s="11"/>
+      <c r="J47" s="11">
+        <v>6952101001</v>
+      </c>
+      <c r="K47" s="12">
         <v>43990</v>
       </c>
-      <c r="L47" s="14">
+      <c r="L47" s="13">
         <v>0.65848379629629628</v>
       </c>
-      <c r="M47" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="N47" s="12" t="s">
+      <c r="M47" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="N47" s="11" t="s">
         <v>51</v>
       </c>
       <c r="O47" s="4"/>
@@ -2980,42 +2987,42 @@
       <c r="V47" s="4"/>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="s">
+      <c r="A48" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B48" s="9">
-        <v>211</v>
-      </c>
-      <c r="C48" s="9">
+      <c r="B48" s="8">
+        <v>211</v>
+      </c>
+      <c r="C48" s="8">
         <v>12312274</v>
       </c>
-      <c r="D48" s="9" t="s">
+      <c r="D48" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E48" s="9">
-        <v>104</v>
-      </c>
-      <c r="F48" s="9">
+      <c r="E48" s="8">
+        <v>104</v>
+      </c>
+      <c r="F48" s="8">
         <v>20018594</v>
       </c>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9" t="s">
+      <c r="G48" s="8"/>
+      <c r="H48" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="I48" s="9"/>
-      <c r="J48" s="9">
-        <v>6952101001</v>
-      </c>
-      <c r="K48" s="10">
+      <c r="I48" s="8"/>
+      <c r="J48" s="8">
+        <v>6952101001</v>
+      </c>
+      <c r="K48" s="9">
         <v>43990</v>
       </c>
-      <c r="L48" s="11">
+      <c r="L48" s="10">
         <v>0.66003472222222226</v>
       </c>
-      <c r="M48" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="N48" s="9" t="s">
+      <c r="M48" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N48" s="8" t="s">
         <v>56</v>
       </c>
       <c r="O48" s="4"/>
@@ -3028,42 +3035,42 @@
       <c r="V48" s="4"/>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B49" s="12">
-        <v>211</v>
-      </c>
-      <c r="C49" s="12">
+      <c r="B49" s="11">
+        <v>211</v>
+      </c>
+      <c r="C49" s="11">
         <v>15283381</v>
       </c>
-      <c r="D49" s="12" t="s">
+      <c r="D49" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E49" s="12">
+      <c r="E49" s="11">
         <v>110</v>
       </c>
-      <c r="F49" s="12">
+      <c r="F49" s="11">
         <v>20018595</v>
       </c>
-      <c r="G49" s="12"/>
-      <c r="H49" s="12" t="s">
+      <c r="G49" s="11"/>
+      <c r="H49" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="I49" s="12"/>
-      <c r="J49" s="12">
-        <v>6952101001</v>
-      </c>
-      <c r="K49" s="13">
+      <c r="I49" s="11"/>
+      <c r="J49" s="11">
+        <v>6952101001</v>
+      </c>
+      <c r="K49" s="12">
         <v>43990</v>
       </c>
-      <c r="L49" s="14">
+      <c r="L49" s="13">
         <v>0.6607291666666667</v>
       </c>
-      <c r="M49" s="12" t="s">
+      <c r="M49" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="N49" s="12" t="s">
+      <c r="N49" s="11" t="s">
         <v>51</v>
       </c>
       <c r="O49" s="4"/>
@@ -3076,42 +3083,42 @@
       <c r="V49" s="4"/>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A50" s="16" t="s">
+      <c r="A50" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B50" s="9">
-        <v>211</v>
-      </c>
-      <c r="C50" s="9">
+      <c r="B50" s="8">
+        <v>211</v>
+      </c>
+      <c r="C50" s="8">
         <v>19130584</v>
       </c>
-      <c r="D50" s="9" t="s">
+      <c r="D50" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E50" s="9">
+      <c r="E50" s="8">
         <v>110</v>
       </c>
-      <c r="F50" s="9">
+      <c r="F50" s="8">
         <v>20018595</v>
       </c>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9" t="s">
+      <c r="G50" s="8"/>
+      <c r="H50" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="I50" s="9"/>
-      <c r="J50" s="9">
-        <v>6952101001</v>
-      </c>
-      <c r="K50" s="10">
+      <c r="I50" s="8"/>
+      <c r="J50" s="8">
+        <v>6952101001</v>
+      </c>
+      <c r="K50" s="9">
         <v>43990</v>
       </c>
-      <c r="L50" s="11">
+      <c r="L50" s="10">
         <v>0.66142361111111114</v>
       </c>
-      <c r="M50" s="9" t="s">
+      <c r="M50" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="N50" s="9" t="s">
+      <c r="N50" s="8" t="s">
         <v>51</v>
       </c>
       <c r="O50" s="4"/>
@@ -3124,42 +3131,42 @@
       <c r="V50" s="4"/>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A51" s="15" t="s">
+      <c r="A51" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B51" s="12">
-        <v>211</v>
-      </c>
-      <c r="C51" s="12">
+      <c r="B51" s="11">
+        <v>211</v>
+      </c>
+      <c r="C51" s="11">
         <v>19130584</v>
       </c>
-      <c r="D51" s="12" t="s">
+      <c r="D51" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E51" s="12">
-        <v>104</v>
-      </c>
-      <c r="F51" s="12">
+      <c r="E51" s="11">
+        <v>104</v>
+      </c>
+      <c r="F51" s="11">
         <v>20018595</v>
       </c>
-      <c r="G51" s="12"/>
-      <c r="H51" s="12" t="s">
+      <c r="G51" s="11"/>
+      <c r="H51" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I51" s="12"/>
-      <c r="J51" s="12">
-        <v>6952101001</v>
-      </c>
-      <c r="K51" s="13">
+      <c r="I51" s="11"/>
+      <c r="J51" s="11">
+        <v>6952101001</v>
+      </c>
+      <c r="K51" s="12">
         <v>43990</v>
       </c>
-      <c r="L51" s="14">
+      <c r="L51" s="13">
         <v>0.66211805555555558</v>
       </c>
-      <c r="M51" s="12" t="s">
+      <c r="M51" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="N51" s="12" t="s">
+      <c r="N51" s="11" t="s">
         <v>51</v>
       </c>
       <c r="O51" s="4"/>
@@ -3172,42 +3179,42 @@
       <c r="V51" s="4"/>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A52" s="16" t="s">
+      <c r="A52" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B52" s="9">
-        <v>211</v>
-      </c>
-      <c r="C52" s="9">
+      <c r="B52" s="8">
+        <v>211</v>
+      </c>
+      <c r="C52" s="8">
         <v>19130584</v>
       </c>
-      <c r="D52" s="9" t="s">
+      <c r="D52" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E52" s="9">
-        <v>104</v>
-      </c>
-      <c r="F52" s="9">
+      <c r="E52" s="8">
+        <v>104</v>
+      </c>
+      <c r="F52" s="8">
         <v>20018595</v>
       </c>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9" t="s">
+      <c r="G52" s="8"/>
+      <c r="H52" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="I52" s="9"/>
-      <c r="J52" s="9">
-        <v>6952101001</v>
-      </c>
-      <c r="K52" s="10">
+      <c r="I52" s="8"/>
+      <c r="J52" s="8">
+        <v>6952101001</v>
+      </c>
+      <c r="K52" s="9">
         <v>43990</v>
       </c>
-      <c r="L52" s="11">
+      <c r="L52" s="10">
         <v>0.66281250000000003</v>
       </c>
-      <c r="M52" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="N52" s="9" t="s">
+      <c r="M52" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N52" s="8" t="s">
         <v>51</v>
       </c>
       <c r="O52" s="4"/>
@@ -3220,42 +3227,42 @@
       <c r="V52" s="4"/>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A53" s="15" t="s">
+      <c r="A53" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B53" s="12">
-        <v>211</v>
-      </c>
-      <c r="C53" s="12">
+      <c r="B53" s="11">
+        <v>211</v>
+      </c>
+      <c r="C53" s="11">
         <v>12312274</v>
       </c>
-      <c r="D53" s="12" t="s">
+      <c r="D53" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E53" s="12">
-        <v>104</v>
-      </c>
-      <c r="F53" s="12">
+      <c r="E53" s="11">
+        <v>104</v>
+      </c>
+      <c r="F53" s="11">
         <v>20018595</v>
       </c>
-      <c r="G53" s="12"/>
-      <c r="H53" s="12" t="s">
+      <c r="G53" s="11"/>
+      <c r="H53" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="I53" s="12"/>
-      <c r="J53" s="12">
-        <v>6952101001</v>
-      </c>
-      <c r="K53" s="13">
+      <c r="I53" s="11"/>
+      <c r="J53" s="11">
+        <v>6952101001</v>
+      </c>
+      <c r="K53" s="12">
         <v>43990</v>
       </c>
-      <c r="L53" s="14">
+      <c r="L53" s="13">
         <v>0.66350694444444447</v>
       </c>
-      <c r="M53" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="N53" s="12" t="s">
+      <c r="M53" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="N53" s="11" t="s">
         <v>56</v>
       </c>
       <c r="O53" s="4"/>
@@ -3268,42 +3275,42 @@
       <c r="V53" s="4"/>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A54" s="16" t="s">
+      <c r="A54" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B54" s="9">
-        <v>211</v>
-      </c>
-      <c r="C54" s="9">
+      <c r="B54" s="8">
+        <v>211</v>
+      </c>
+      <c r="C54" s="8">
         <v>19130584</v>
       </c>
-      <c r="D54" s="9" t="s">
+      <c r="D54" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E54" s="9">
-        <v>104</v>
-      </c>
-      <c r="F54" s="9">
+      <c r="E54" s="8">
+        <v>104</v>
+      </c>
+      <c r="F54" s="8">
         <v>20018596</v>
       </c>
-      <c r="G54" s="9"/>
-      <c r="H54" s="9" t="s">
+      <c r="G54" s="8"/>
+      <c r="H54" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="I54" s="9"/>
-      <c r="J54" s="9">
-        <v>6952101001</v>
-      </c>
-      <c r="K54" s="10">
+      <c r="I54" s="8"/>
+      <c r="J54" s="8">
+        <v>6952101001</v>
+      </c>
+      <c r="K54" s="9">
         <v>43990</v>
       </c>
-      <c r="L54" s="11">
+      <c r="L54" s="10">
         <v>0.66403935185185181</v>
       </c>
-      <c r="M54" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="N54" s="9" t="s">
+      <c r="M54" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N54" s="8" t="s">
         <v>51</v>
       </c>
       <c r="O54" s="4"/>
@@ -3316,42 +3323,42 @@
       <c r="V54" s="4"/>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A55" s="15" t="s">
+      <c r="A55" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B55" s="12">
-        <v>211</v>
-      </c>
-      <c r="C55" s="12">
+      <c r="B55" s="11">
+        <v>211</v>
+      </c>
+      <c r="C55" s="11">
         <v>12312274</v>
       </c>
-      <c r="D55" s="12" t="s">
+      <c r="D55" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E55" s="12">
-        <v>104</v>
-      </c>
-      <c r="F55" s="12">
+      <c r="E55" s="11">
+        <v>104</v>
+      </c>
+      <c r="F55" s="11">
         <v>20018596</v>
       </c>
-      <c r="G55" s="12"/>
-      <c r="H55" s="12" t="s">
+      <c r="G55" s="11"/>
+      <c r="H55" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="I55" s="12"/>
-      <c r="J55" s="12">
-        <v>6952101001</v>
-      </c>
-      <c r="K55" s="13">
+      <c r="I55" s="11"/>
+      <c r="J55" s="11">
+        <v>6952101001</v>
+      </c>
+      <c r="K55" s="12">
         <v>43990</v>
       </c>
-      <c r="L55" s="14">
+      <c r="L55" s="13">
         <v>0.66489583333333335</v>
       </c>
-      <c r="M55" s="12" t="s">
+      <c r="M55" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="N55" s="12" t="s">
+      <c r="N55" s="11" t="s">
         <v>56</v>
       </c>
       <c r="O55" s="4"/>
@@ -3364,42 +3371,42 @@
       <c r="V55" s="4"/>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A56" s="16" t="s">
+      <c r="A56" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B56" s="9">
-        <v>211</v>
-      </c>
-      <c r="C56" s="9">
+      <c r="B56" s="8">
+        <v>211</v>
+      </c>
+      <c r="C56" s="8">
         <v>12312274</v>
       </c>
-      <c r="D56" s="9" t="s">
+      <c r="D56" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E56" s="9">
-        <v>104</v>
-      </c>
-      <c r="F56" s="9">
+      <c r="E56" s="8">
+        <v>104</v>
+      </c>
+      <c r="F56" s="8">
         <v>20018596</v>
       </c>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9" t="s">
+      <c r="G56" s="8"/>
+      <c r="H56" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="I56" s="9"/>
-      <c r="J56" s="9">
-        <v>6952101001</v>
-      </c>
-      <c r="K56" s="10">
+      <c r="I56" s="8"/>
+      <c r="J56" s="8">
+        <v>6952101001</v>
+      </c>
+      <c r="K56" s="9">
         <v>43990</v>
       </c>
-      <c r="L56" s="11">
+      <c r="L56" s="10">
         <v>0.66559027777777779</v>
       </c>
-      <c r="M56" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="N56" s="9" t="s">
+      <c r="M56" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N56" s="8" t="s">
         <v>56</v>
       </c>
       <c r="O56" s="4"/>
@@ -3412,42 +3419,42 @@
       <c r="V56" s="4"/>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A57" s="15" t="s">
+      <c r="A57" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B57" s="12">
-        <v>211</v>
-      </c>
-      <c r="C57" s="12">
+      <c r="B57" s="11">
+        <v>211</v>
+      </c>
+      <c r="C57" s="11">
         <v>19130584</v>
       </c>
-      <c r="D57" s="12" t="s">
+      <c r="D57" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E57" s="12">
-        <v>104</v>
-      </c>
-      <c r="F57" s="12">
+      <c r="E57" s="11">
+        <v>104</v>
+      </c>
+      <c r="F57" s="11">
         <v>20018597</v>
       </c>
-      <c r="G57" s="12"/>
-      <c r="H57" s="12" t="s">
+      <c r="G57" s="11"/>
+      <c r="H57" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I57" s="12"/>
-      <c r="J57" s="12">
-        <v>6952101001</v>
-      </c>
-      <c r="K57" s="13">
+      <c r="I57" s="11"/>
+      <c r="J57" s="11">
+        <v>6952101001</v>
+      </c>
+      <c r="K57" s="12">
         <v>43990</v>
       </c>
-      <c r="L57" s="14">
+      <c r="L57" s="13">
         <v>0.66612268518518525</v>
       </c>
-      <c r="M57" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="N57" s="12" t="s">
+      <c r="M57" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="N57" s="11" t="s">
         <v>51</v>
       </c>
       <c r="O57" s="4"/>
@@ -3460,42 +3467,42 @@
       <c r="V57" s="4"/>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A58" s="16" t="s">
+      <c r="A58" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B58" s="9">
-        <v>211</v>
-      </c>
-      <c r="C58" s="9">
+      <c r="B58" s="8">
+        <v>211</v>
+      </c>
+      <c r="C58" s="8">
         <v>12312274</v>
       </c>
-      <c r="D58" s="9" t="s">
+      <c r="D58" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E58" s="9">
-        <v>104</v>
-      </c>
-      <c r="F58" s="9">
+      <c r="E58" s="8">
+        <v>104</v>
+      </c>
+      <c r="F58" s="8">
         <v>20018597</v>
       </c>
-      <c r="G58" s="9"/>
-      <c r="H58" s="9" t="s">
+      <c r="G58" s="8"/>
+      <c r="H58" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="I58" s="9"/>
-      <c r="J58" s="9">
-        <v>6952101001</v>
-      </c>
-      <c r="K58" s="10">
+      <c r="I58" s="8"/>
+      <c r="J58" s="8">
+        <v>6952101001</v>
+      </c>
+      <c r="K58" s="9">
         <v>43990</v>
       </c>
-      <c r="L58" s="11">
+      <c r="L58" s="10">
         <v>0.66697916666666668</v>
       </c>
-      <c r="M58" s="9" t="s">
+      <c r="M58" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="N58" s="9" t="s">
+      <c r="N58" s="8" t="s">
         <v>56</v>
       </c>
       <c r="O58" s="4"/>
@@ -3508,42 +3515,42 @@
       <c r="V58" s="4"/>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A59" s="15" t="s">
+      <c r="A59" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B59" s="12">
-        <v>211</v>
-      </c>
-      <c r="C59" s="12">
+      <c r="B59" s="11">
+        <v>211</v>
+      </c>
+      <c r="C59" s="11">
         <v>12312274</v>
       </c>
-      <c r="D59" s="12" t="s">
+      <c r="D59" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E59" s="12">
-        <v>104</v>
-      </c>
-      <c r="F59" s="12">
+      <c r="E59" s="11">
+        <v>104</v>
+      </c>
+      <c r="F59" s="11">
         <v>20018597</v>
       </c>
-      <c r="G59" s="12"/>
-      <c r="H59" s="12" t="s">
+      <c r="G59" s="11"/>
+      <c r="H59" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="I59" s="12"/>
-      <c r="J59" s="12">
-        <v>6952101001</v>
-      </c>
-      <c r="K59" s="13">
+      <c r="I59" s="11"/>
+      <c r="J59" s="11">
+        <v>6952101001</v>
+      </c>
+      <c r="K59" s="12">
         <v>43990</v>
       </c>
-      <c r="L59" s="14">
+      <c r="L59" s="13">
         <v>0.66767361111111112</v>
       </c>
-      <c r="M59" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="N59" s="12" t="s">
+      <c r="M59" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="N59" s="11" t="s">
         <v>56</v>
       </c>
       <c r="O59" s="4"/>
@@ -3556,42 +3563,42 @@
       <c r="V59" s="4"/>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A60" s="16" t="s">
+      <c r="A60" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B60" s="9">
-        <v>211</v>
-      </c>
-      <c r="C60" s="9">
+      <c r="B60" s="8">
+        <v>211</v>
+      </c>
+      <c r="C60" s="8">
         <v>19130584</v>
       </c>
-      <c r="D60" s="9" t="s">
+      <c r="D60" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E60" s="9">
-        <v>104</v>
-      </c>
-      <c r="F60" s="9">
+      <c r="E60" s="8">
+        <v>104</v>
+      </c>
+      <c r="F60" s="8">
         <v>20018598</v>
       </c>
-      <c r="G60" s="9"/>
-      <c r="H60" s="9" t="s">
+      <c r="G60" s="8"/>
+      <c r="H60" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="I60" s="9"/>
-      <c r="J60" s="9">
-        <v>6952101001</v>
-      </c>
-      <c r="K60" s="10">
+      <c r="I60" s="8"/>
+      <c r="J60" s="8">
+        <v>6952101001</v>
+      </c>
+      <c r="K60" s="9">
         <v>43990</v>
       </c>
-      <c r="L60" s="11">
+      <c r="L60" s="10">
         <v>0.66820601851851846</v>
       </c>
-      <c r="M60" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="N60" s="9" t="s">
+      <c r="M60" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N60" s="8" t="s">
         <v>51</v>
       </c>
       <c r="O60" s="4"/>
@@ -3604,42 +3611,42 @@
       <c r="V60" s="4"/>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A61" s="15" t="s">
+      <c r="A61" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B61" s="12">
-        <v>211</v>
-      </c>
-      <c r="C61" s="12">
+      <c r="B61" s="11">
+        <v>211</v>
+      </c>
+      <c r="C61" s="11">
         <v>12312274</v>
       </c>
-      <c r="D61" s="12" t="s">
+      <c r="D61" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E61" s="12">
-        <v>104</v>
-      </c>
-      <c r="F61" s="12">
+      <c r="E61" s="11">
+        <v>104</v>
+      </c>
+      <c r="F61" s="11">
         <v>20018598</v>
       </c>
-      <c r="G61" s="12"/>
-      <c r="H61" s="12" t="s">
+      <c r="G61" s="11"/>
+      <c r="H61" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="I61" s="12"/>
-      <c r="J61" s="12">
-        <v>6952101001</v>
-      </c>
-      <c r="K61" s="13">
+      <c r="I61" s="11"/>
+      <c r="J61" s="11">
+        <v>6952101001</v>
+      </c>
+      <c r="K61" s="12">
         <v>43990</v>
       </c>
-      <c r="L61" s="14">
+      <c r="L61" s="13">
         <v>0.6690625</v>
       </c>
-      <c r="M61" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="N61" s="12" t="s">
+      <c r="M61" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="N61" s="11" t="s">
         <v>56</v>
       </c>
       <c r="O61" s="4"/>
@@ -3652,42 +3659,42 @@
       <c r="V61" s="4"/>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A62" s="16" t="s">
+      <c r="A62" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B62" s="9">
-        <v>211</v>
-      </c>
-      <c r="C62" s="9">
+      <c r="B62" s="8">
+        <v>211</v>
+      </c>
+      <c r="C62" s="8">
         <v>19130584</v>
       </c>
-      <c r="D62" s="9" t="s">
+      <c r="D62" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E62" s="9">
-        <v>104</v>
-      </c>
-      <c r="F62" s="9">
+      <c r="E62" s="8">
+        <v>104</v>
+      </c>
+      <c r="F62" s="8">
         <v>20018599</v>
       </c>
-      <c r="G62" s="9"/>
-      <c r="H62" s="9" t="s">
+      <c r="G62" s="8"/>
+      <c r="H62" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="I62" s="9"/>
-      <c r="J62" s="9">
-        <v>6952101001</v>
-      </c>
-      <c r="K62" s="10">
+      <c r="I62" s="8"/>
+      <c r="J62" s="8">
+        <v>6952101001</v>
+      </c>
+      <c r="K62" s="9">
         <v>43990</v>
       </c>
-      <c r="L62" s="11">
+      <c r="L62" s="10">
         <v>0.66820601851851846</v>
       </c>
-      <c r="M62" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="N62" s="9" t="s">
+      <c r="M62" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N62" s="8" t="s">
         <v>51</v>
       </c>
       <c r="O62" s="4"/>
@@ -3700,42 +3707,42 @@
       <c r="V62" s="4"/>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A63" s="17" t="s">
+      <c r="A63" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B63" s="18">
-        <v>211</v>
-      </c>
-      <c r="C63" s="18">
+      <c r="B63" s="17">
+        <v>211</v>
+      </c>
+      <c r="C63" s="17">
         <v>12312274</v>
       </c>
-      <c r="D63" s="18" t="s">
+      <c r="D63" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="E63" s="18">
-        <v>104</v>
-      </c>
-      <c r="F63" s="18">
+      <c r="E63" s="17">
+        <v>104</v>
+      </c>
+      <c r="F63" s="17">
         <v>20018599</v>
       </c>
-      <c r="G63" s="18"/>
-      <c r="H63" s="18" t="s">
+      <c r="G63" s="17"/>
+      <c r="H63" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="I63" s="18"/>
-      <c r="J63" s="18">
-        <v>6952101001</v>
-      </c>
-      <c r="K63" s="19">
+      <c r="I63" s="17"/>
+      <c r="J63" s="17">
+        <v>6952101001</v>
+      </c>
+      <c r="K63" s="18">
         <v>43990</v>
       </c>
-      <c r="L63" s="20">
+      <c r="L63" s="19">
         <v>0.6690625</v>
       </c>
-      <c r="M63" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="N63" s="18" t="s">
+      <c r="M63" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="N63" s="17" t="s">
         <v>56</v>
       </c>
       <c r="O63" s="4"/>
@@ -4733,21 +4740,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -4841,4 +4848,171 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D2:F24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="8">
+        <v>20118589</v>
+      </c>
+      <c r="F3" s="8">
+        <v>20118590</v>
+      </c>
+    </row>
+    <row r="4" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D4" s="8">
+        <v>20118595</v>
+      </c>
+      <c r="F4" s="11">
+        <v>20118591</v>
+      </c>
+    </row>
+    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D5" s="11">
+        <v>20118596</v>
+      </c>
+      <c r="F5" s="8">
+        <v>20118592</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D6" s="8">
+        <v>20118597</v>
+      </c>
+      <c r="F6" s="11">
+        <v>20118593</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="8">
+        <v>20018589</v>
+      </c>
+      <c r="F7" s="11">
+        <v>20118594</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="11">
+        <v>20018595</v>
+      </c>
+      <c r="F8" s="11">
+        <v>20118598</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="8">
+        <v>20018596</v>
+      </c>
+      <c r="F9" s="11">
+        <v>20118599</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="8">
+        <v>20018597</v>
+      </c>
+      <c r="F10" s="11">
+        <v>20018590</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="11">
+        <v>20102326</v>
+      </c>
+      <c r="F11" s="11">
+        <v>20018591</v>
+      </c>
+    </row>
+    <row r="12" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="11">
+        <v>20102327</v>
+      </c>
+      <c r="F12" s="11">
+        <v>20018592</v>
+      </c>
+    </row>
+    <row r="13" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="11">
+        <v>20018593</v>
+      </c>
+    </row>
+    <row r="14" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="8">
+        <v>20018594</v>
+      </c>
+    </row>
+    <row r="15" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="11">
+        <v>20018598</v>
+      </c>
+    </row>
+    <row r="16" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="8">
+        <v>20018599</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="8">
+        <v>20102318</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="8">
+        <v>20102319</v>
+      </c>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="8">
+        <v>20102320</v>
+      </c>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="8">
+        <v>20102321</v>
+      </c>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F21" s="8">
+        <v>20102322</v>
+      </c>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="8">
+        <v>20102323</v>
+      </c>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="8">
+        <v>20102324</v>
+      </c>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="8">
+        <v>20102325</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>